<commit_message>
Version : V0.1.15 ChangeLog : 1.Dcm_TypeStack ： add some definition. 2.Dcm : fix the bugs,the Dsp_UdsServiceCtrInfo[ChNo].ReqDL write error in Dcm_RxDiagRequestInfo function. 3.Dcm : in Dcm_RxDiagRequestInfo function add check the services is support sub-function check. 4.Dsp : add Dsp_CheckServicesIsSupportSubFunction function,used for check the services if support the sub-function. 5.Dsp : add Dsp_ServicesFunction_ClearDiagnosticInformation function,used implements the $14 server. 6.Dcm_Table : add Dsp_Services_0x14_SupportFunctionList,used for 14 service configuration parameters----not debug. 7.Dsp : add Dsp_CheckDTCGroupTypeOfClearDiagnosticInformationIsSupport,used for check the Dtc group is support. 8.Tools : update 14 service configuration attribute. Autor : Mingfen XIAO(mingfen.xiao@qq.com) Data  : 2018.12.17
</commit_message>
<xml_diff>
--- a/01_Documents/04_ConfigurationTools/DiagnosticStack_ConfigurationTools.xlsx
+++ b/01_Documents/04_ConfigurationTools/DiagnosticStack_ConfigurationTools.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="831" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="831" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="00_Cover" sheetId="5" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'02_SecurityAccess'!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
   <si>
     <t>DefaultSession</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -336,14 +337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0xFFFFFF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All Group</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P2*Server_max
 (Resolution:1ms)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -389,6 +382,67 @@
 2.add Sheet 00_ChanageLog
 3.Modify 00_Cover:
   ChanageLog form modified to ReleaseNote</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mingfen XIAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Modified 06_DiagnosticService_0x14 sheet:add note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.12.17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubFunction Identifier(Hex)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(U)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(P)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note:
+1.The service not support sub function.
+2.The table SubFunctionIdentifier(Hex) column value not indication the services SubFunctionIdentifier.Its means:
+  Emission-related System(E)   bit0
+  Powertrain(P)                bit1
+  Chassis(C)                   bit2
+  Body(B)                      bit3
+  Network(U)                   bit4
+  All Group(A)                 bit5
+  Each DTCs(O)                 bit6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(O)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(E)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -399,7 +453,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,8 +571,17 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,8 +594,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -753,6 +822,204 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -762,7 +1029,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -922,6 +1189,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -948,6 +1260,18 @@
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -979,40 +1303,55 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1899,56 +2238,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
     </row>
     <row r="3" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
@@ -1968,15 +2307,15 @@
       <c r="C7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="59"/>
+      <c r="D7" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="74"/>
       <c r="F7" s="33" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H7" s="18"/>
     </row>
@@ -1984,11 +2323,11 @@
       <c r="A8" s="18"/>
       <c r="B8" s="34"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H8" s="18"/>
     </row>
@@ -1996,8 +2335,8 @@
       <c r="A9" s="18"/>
       <c r="B9" s="34"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="72"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="18"/>
@@ -2006,8 +2345,8 @@
       <c r="A10" s="18"/>
       <c r="B10" s="34"/>
       <c r="C10" s="16"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
       <c r="H10" s="18"/>
@@ -2016,8 +2355,8 @@
       <c r="A11" s="18"/>
       <c r="B11" s="34"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="H11" s="18"/>
@@ -2026,8 +2365,8 @@
       <c r="A12" s="18"/>
       <c r="B12" s="34"/>
       <c r="C12" s="16"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="57"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="72"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="18"/>
@@ -2036,8 +2375,8 @@
       <c r="A13" s="18"/>
       <c r="B13" s="34"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="57"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
       <c r="H13" s="18"/>
@@ -2046,8 +2385,8 @@
       <c r="A14" s="18"/>
       <c r="B14" s="34"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
       <c r="H14" s="18"/>
@@ -2056,8 +2395,8 @@
       <c r="A15" s="18"/>
       <c r="B15" s="34"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
       <c r="H15" s="18"/>
@@ -2066,8 +2405,8 @@
       <c r="A16" s="18"/>
       <c r="B16" s="34"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
       <c r="H16" s="18"/>
@@ -2076,8 +2415,8 @@
       <c r="A17" s="18"/>
       <c r="B17" s="34"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
       <c r="H17" s="18"/>
@@ -2086,8 +2425,8 @@
       <c r="A18" s="18"/>
       <c r="B18" s="34"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
       <c r="H18" s="18"/>
@@ -2096,8 +2435,8 @@
       <c r="A19" s="18"/>
       <c r="B19" s="34"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="57"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="35"/>
       <c r="G19" s="35"/>
       <c r="H19" s="18"/>
@@ -2106,8 +2445,8 @@
       <c r="A20" s="18"/>
       <c r="B20" s="34"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="72"/>
       <c r="F20" s="35"/>
       <c r="G20" s="35"/>
       <c r="H20" s="18"/>
@@ -2116,8 +2455,8 @@
       <c r="A21" s="18"/>
       <c r="B21" s="34"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="35"/>
       <c r="G21" s="35"/>
       <c r="H21" s="18"/>
@@ -2126,8 +2465,8 @@
       <c r="A22" s="18"/>
       <c r="B22" s="34"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="72"/>
       <c r="F22" s="35"/>
       <c r="G22" s="35"/>
       <c r="H22" s="18"/>
@@ -2136,8 +2475,8 @@
       <c r="A23" s="18"/>
       <c r="B23" s="34"/>
       <c r="C23" s="16"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="35"/>
       <c r="G23" s="35"/>
       <c r="H23" s="18"/>
@@ -2146,8 +2485,8 @@
       <c r="A24" s="18"/>
       <c r="B24" s="34"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="57"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="72"/>
       <c r="F24" s="35"/>
       <c r="G24" s="35"/>
       <c r="H24" s="18"/>
@@ -2156,8 +2495,8 @@
       <c r="A25" s="18"/>
       <c r="B25" s="36"/>
       <c r="C25" s="37"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="76"/>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
       <c r="H25" s="18"/>
@@ -2173,26 +2512,26 @@
       <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
     </row>
     <row r="28" spans="1:8" s="21" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
     </row>
     <row r="29" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="22"/>
@@ -3196,41 +3535,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:E14"/>
+    <sheetView view="pageBreakPreview" zoomScale="190" zoomScaleNormal="160" zoomScaleSheetLayoutView="190" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.875" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="B2" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="80"/>
-    </row>
-    <row r="3" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="81" t="s">
+      <c r="B2" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="79"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B3" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="82" t="s">
+      <c r="D3" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="80"/>
+      <c r="F3" s="60" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3241,916 +3581,924 @@
       <c r="C4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="72"/>
+      <c r="F5" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="56" t="s">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B6" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="57"/>
-      <c r="F5" s="35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="34"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="35"/>
+      <c r="D6" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="72"/>
+      <c r="F6" s="35" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B7" s="34"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="72"/>
       <c r="F7" s="35"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B8" s="34"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
       <c r="F8" s="35"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B9" s="34"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="72"/>
       <c r="F9" s="35"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B10" s="34"/>
       <c r="C10" s="16"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="35"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B11" s="34"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72"/>
       <c r="F11" s="35"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B12" s="34"/>
       <c r="C12" s="16"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="57"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="72"/>
       <c r="F12" s="35"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B13" s="34"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="57"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="35"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B14" s="34"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="35"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B15" s="34"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="35"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B16" s="34"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="35"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B17" s="34"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="35"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B18" s="34"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="35"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B19" s="34"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="57"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="35"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B20" s="34"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="72"/>
       <c r="F20" s="35"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B21" s="34"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="35"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B22" s="34"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="72"/>
       <c r="F22" s="35"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B23" s="34"/>
       <c r="C23" s="16"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="35"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B24" s="34"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="57"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="72"/>
       <c r="F24" s="35"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B25" s="34"/>
       <c r="C25" s="16"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="57"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="72"/>
       <c r="F25" s="35"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B26" s="34"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="72"/>
       <c r="F26" s="35"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="34"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="35"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B28" s="34"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="72"/>
       <c r="F28" s="35"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B29" s="34"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="35"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B30" s="34"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="57"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="72"/>
       <c r="F30" s="35"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B31" s="34"/>
       <c r="C31" s="16"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="72"/>
       <c r="F31" s="35"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B32" s="34"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="57"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="72"/>
       <c r="F32" s="35"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="34"/>
       <c r="C33" s="16"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="72"/>
       <c r="F33" s="35"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B34" s="34"/>
       <c r="C34" s="16"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="72"/>
       <c r="F34" s="35"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B35" s="34"/>
       <c r="C35" s="16"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="57"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="72"/>
       <c r="F35" s="35"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B36" s="34"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="72"/>
       <c r="F36" s="35"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B37" s="34"/>
       <c r="C37" s="16"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="57"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="72"/>
       <c r="F37" s="35"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B38" s="34"/>
       <c r="C38" s="16"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="57"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="35"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B39" s="34"/>
       <c r="C39" s="16"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="57"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="72"/>
       <c r="F39" s="35"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B40" s="34"/>
       <c r="C40" s="16"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="57"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="72"/>
       <c r="F40" s="35"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B41" s="34"/>
       <c r="C41" s="16"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="57"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="35"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B42" s="34"/>
       <c r="C42" s="16"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="57"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="72"/>
       <c r="F42" s="35"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B43" s="34"/>
       <c r="C43" s="16"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="57"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="72"/>
       <c r="F43" s="35"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B44" s="34"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="57"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="72"/>
       <c r="F44" s="35"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B45" s="34"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="57"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="72"/>
       <c r="F45" s="35"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B46" s="34"/>
       <c r="C46" s="16"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="57"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="35"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B47" s="34"/>
       <c r="C47" s="16"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="57"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="35"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B48" s="34"/>
       <c r="C48" s="16"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="57"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="72"/>
       <c r="F48" s="35"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B49" s="34"/>
       <c r="C49" s="16"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="57"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="72"/>
       <c r="F49" s="35"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B50" s="34"/>
       <c r="C50" s="16"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="57"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="72"/>
       <c r="F50" s="35"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B51" s="34"/>
       <c r="C51" s="16"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="57"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="72"/>
       <c r="F51" s="35"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B52" s="34"/>
       <c r="C52" s="16"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="57"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="72"/>
       <c r="F52" s="35"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B53" s="34"/>
       <c r="C53" s="16"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="57"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="72"/>
       <c r="F53" s="35"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B54" s="34"/>
       <c r="C54" s="16"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="57"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="72"/>
       <c r="F54" s="35"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B55" s="34"/>
       <c r="C55" s="16"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="57"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="72"/>
       <c r="F55" s="35"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B56" s="34"/>
       <c r="C56" s="16"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="57"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="72"/>
       <c r="F56" s="35"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B57" s="34"/>
       <c r="C57" s="16"/>
-      <c r="D57" s="56"/>
-      <c r="E57" s="57"/>
+      <c r="D57" s="71"/>
+      <c r="E57" s="72"/>
       <c r="F57" s="35"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B58" s="34"/>
       <c r="C58" s="16"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="57"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="72"/>
       <c r="F58" s="35"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B59" s="34"/>
       <c r="C59" s="16"/>
-      <c r="D59" s="56"/>
-      <c r="E59" s="57"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="35"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B60" s="34"/>
       <c r="C60" s="16"/>
-      <c r="D60" s="56"/>
-      <c r="E60" s="57"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="72"/>
       <c r="F60" s="35"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B61" s="34"/>
       <c r="C61" s="16"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="57"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="72"/>
       <c r="F61" s="35"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B62" s="34"/>
       <c r="C62" s="16"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="57"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="72"/>
       <c r="F62" s="35"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B63" s="34"/>
       <c r="C63" s="16"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="57"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="72"/>
       <c r="F63" s="35"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B64" s="34"/>
       <c r="C64" s="16"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="57"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="72"/>
       <c r="F64" s="35"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B65" s="34"/>
       <c r="C65" s="16"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="57"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="72"/>
       <c r="F65" s="35"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B66" s="34"/>
       <c r="C66" s="16"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="57"/>
+      <c r="D66" s="71"/>
+      <c r="E66" s="72"/>
       <c r="F66" s="35"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B67" s="34"/>
       <c r="C67" s="16"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="57"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="72"/>
       <c r="F67" s="35"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B68" s="34"/>
       <c r="C68" s="16"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="57"/>
+      <c r="D68" s="71"/>
+      <c r="E68" s="72"/>
       <c r="F68" s="35"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B69" s="34"/>
       <c r="C69" s="16"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="57"/>
+      <c r="D69" s="71"/>
+      <c r="E69" s="72"/>
       <c r="F69" s="35"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B70" s="34"/>
       <c r="C70" s="16"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="57"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="72"/>
       <c r="F70" s="35"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B71" s="34"/>
       <c r="C71" s="16"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="57"/>
+      <c r="D71" s="71"/>
+      <c r="E71" s="72"/>
       <c r="F71" s="35"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B72" s="34"/>
       <c r="C72" s="16"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="57"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="72"/>
       <c r="F72" s="35"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B73" s="34"/>
       <c r="C73" s="16"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="57"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="72"/>
       <c r="F73" s="35"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B74" s="34"/>
       <c r="C74" s="16"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="57"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="72"/>
       <c r="F74" s="35"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B75" s="34"/>
       <c r="C75" s="16"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="57"/>
+      <c r="D75" s="71"/>
+      <c r="E75" s="72"/>
       <c r="F75" s="35"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B76" s="34"/>
       <c r="C76" s="16"/>
-      <c r="D76" s="56"/>
-      <c r="E76" s="57"/>
+      <c r="D76" s="71"/>
+      <c r="E76" s="72"/>
       <c r="F76" s="35"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B77" s="34"/>
       <c r="C77" s="16"/>
-      <c r="D77" s="56"/>
-      <c r="E77" s="57"/>
+      <c r="D77" s="71"/>
+      <c r="E77" s="72"/>
       <c r="F77" s="35"/>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B78" s="34"/>
       <c r="C78" s="16"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="57"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="72"/>
       <c r="F78" s="35"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B79" s="34"/>
       <c r="C79" s="16"/>
-      <c r="D79" s="56"/>
-      <c r="E79" s="57"/>
+      <c r="D79" s="71"/>
+      <c r="E79" s="72"/>
       <c r="F79" s="35"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B80" s="34"/>
       <c r="C80" s="16"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="57"/>
+      <c r="D80" s="71"/>
+      <c r="E80" s="72"/>
       <c r="F80" s="35"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B81" s="34"/>
       <c r="C81" s="16"/>
-      <c r="D81" s="56"/>
-      <c r="E81" s="57"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="72"/>
       <c r="F81" s="35"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B82" s="34"/>
       <c r="C82" s="16"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="57"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="72"/>
       <c r="F82" s="35"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B83" s="34"/>
       <c r="C83" s="16"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="57"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="72"/>
       <c r="F83" s="35"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B84" s="34"/>
       <c r="C84" s="16"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="57"/>
+      <c r="D84" s="71"/>
+      <c r="E84" s="72"/>
       <c r="F84" s="35"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B85" s="34"/>
       <c r="C85" s="16"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="57"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="72"/>
       <c r="F85" s="35"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B86" s="34"/>
       <c r="C86" s="16"/>
-      <c r="D86" s="56"/>
-      <c r="E86" s="57"/>
+      <c r="D86" s="71"/>
+      <c r="E86" s="72"/>
       <c r="F86" s="35"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B87" s="34"/>
       <c r="C87" s="16"/>
-      <c r="D87" s="56"/>
-      <c r="E87" s="57"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="72"/>
       <c r="F87" s="35"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B88" s="34"/>
       <c r="C88" s="16"/>
-      <c r="D88" s="56"/>
-      <c r="E88" s="57"/>
+      <c r="D88" s="71"/>
+      <c r="E88" s="72"/>
       <c r="F88" s="35"/>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B89" s="34"/>
       <c r="C89" s="16"/>
-      <c r="D89" s="56"/>
-      <c r="E89" s="57"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="72"/>
       <c r="F89" s="35"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B90" s="34"/>
       <c r="C90" s="16"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="57"/>
+      <c r="D90" s="71"/>
+      <c r="E90" s="72"/>
       <c r="F90" s="35"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B91" s="34"/>
       <c r="C91" s="16"/>
-      <c r="D91" s="56"/>
-      <c r="E91" s="57"/>
+      <c r="D91" s="71"/>
+      <c r="E91" s="72"/>
       <c r="F91" s="35"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B92" s="34"/>
       <c r="C92" s="16"/>
-      <c r="D92" s="56"/>
-      <c r="E92" s="57"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="72"/>
       <c r="F92" s="35"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B93" s="34"/>
       <c r="C93" s="16"/>
-      <c r="D93" s="56"/>
-      <c r="E93" s="57"/>
+      <c r="D93" s="71"/>
+      <c r="E93" s="72"/>
       <c r="F93" s="35"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B94" s="34"/>
       <c r="C94" s="16"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="57"/>
+      <c r="D94" s="71"/>
+      <c r="E94" s="72"/>
       <c r="F94" s="35"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B95" s="34"/>
       <c r="C95" s="16"/>
-      <c r="D95" s="56"/>
-      <c r="E95" s="57"/>
+      <c r="D95" s="71"/>
+      <c r="E95" s="72"/>
       <c r="F95" s="35"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B96" s="34"/>
       <c r="C96" s="16"/>
-      <c r="D96" s="56"/>
-      <c r="E96" s="57"/>
+      <c r="D96" s="71"/>
+      <c r="E96" s="72"/>
       <c r="F96" s="35"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B97" s="34"/>
       <c r="C97" s="16"/>
-      <c r="D97" s="56"/>
-      <c r="E97" s="57"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="72"/>
       <c r="F97" s="35"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B98" s="34"/>
       <c r="C98" s="16"/>
-      <c r="D98" s="56"/>
-      <c r="E98" s="57"/>
+      <c r="D98" s="71"/>
+      <c r="E98" s="72"/>
       <c r="F98" s="35"/>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B99" s="34"/>
       <c r="C99" s="16"/>
-      <c r="D99" s="56"/>
-      <c r="E99" s="57"/>
+      <c r="D99" s="71"/>
+      <c r="E99" s="72"/>
       <c r="F99" s="35"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B100" s="34"/>
       <c r="C100" s="16"/>
-      <c r="D100" s="56"/>
-      <c r="E100" s="57"/>
+      <c r="D100" s="71"/>
+      <c r="E100" s="72"/>
       <c r="F100" s="35"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B101" s="34"/>
       <c r="C101" s="16"/>
-      <c r="D101" s="56"/>
-      <c r="E101" s="57"/>
+      <c r="D101" s="71"/>
+      <c r="E101" s="72"/>
       <c r="F101" s="35"/>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B102" s="34"/>
       <c r="C102" s="16"/>
-      <c r="D102" s="56"/>
-      <c r="E102" s="57"/>
+      <c r="D102" s="71"/>
+      <c r="E102" s="72"/>
       <c r="F102" s="35"/>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B103" s="34"/>
       <c r="C103" s="16"/>
-      <c r="D103" s="56"/>
-      <c r="E103" s="57"/>
+      <c r="D103" s="71"/>
+      <c r="E103" s="72"/>
       <c r="F103" s="35"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B104" s="34"/>
       <c r="C104" s="16"/>
-      <c r="D104" s="56"/>
-      <c r="E104" s="57"/>
+      <c r="D104" s="71"/>
+      <c r="E104" s="72"/>
       <c r="F104" s="35"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B105" s="34"/>
       <c r="C105" s="16"/>
-      <c r="D105" s="56"/>
-      <c r="E105" s="57"/>
+      <c r="D105" s="71"/>
+      <c r="E105" s="72"/>
       <c r="F105" s="35"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B106" s="34"/>
       <c r="C106" s="16"/>
-      <c r="D106" s="56"/>
-      <c r="E106" s="57"/>
+      <c r="D106" s="71"/>
+      <c r="E106" s="72"/>
       <c r="F106" s="35"/>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B107" s="34"/>
       <c r="C107" s="16"/>
-      <c r="D107" s="56"/>
-      <c r="E107" s="57"/>
+      <c r="D107" s="71"/>
+      <c r="E107" s="72"/>
       <c r="F107" s="35"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B108" s="34"/>
       <c r="C108" s="16"/>
-      <c r="D108" s="56"/>
-      <c r="E108" s="57"/>
+      <c r="D108" s="71"/>
+      <c r="E108" s="72"/>
       <c r="F108" s="35"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B109" s="34"/>
       <c r="C109" s="16"/>
-      <c r="D109" s="56"/>
-      <c r="E109" s="57"/>
+      <c r="D109" s="71"/>
+      <c r="E109" s="72"/>
       <c r="F109" s="35"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B110" s="34"/>
       <c r="C110" s="16"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="57"/>
+      <c r="D110" s="71"/>
+      <c r="E110" s="72"/>
       <c r="F110" s="35"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B111" s="34"/>
       <c r="C111" s="16"/>
-      <c r="D111" s="56"/>
-      <c r="E111" s="57"/>
+      <c r="D111" s="71"/>
+      <c r="E111" s="72"/>
       <c r="F111" s="35"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B112" s="34"/>
       <c r="C112" s="16"/>
-      <c r="D112" s="56"/>
-      <c r="E112" s="57"/>
+      <c r="D112" s="71"/>
+      <c r="E112" s="72"/>
       <c r="F112" s="35"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B113" s="34"/>
       <c r="C113" s="16"/>
-      <c r="D113" s="56"/>
-      <c r="E113" s="57"/>
+      <c r="D113" s="71"/>
+      <c r="E113" s="72"/>
       <c r="F113" s="35"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B114" s="34"/>
       <c r="C114" s="16"/>
-      <c r="D114" s="56"/>
-      <c r="E114" s="57"/>
+      <c r="D114" s="71"/>
+      <c r="E114" s="72"/>
       <c r="F114" s="35"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B115" s="34"/>
       <c r="C115" s="16"/>
-      <c r="D115" s="56"/>
-      <c r="E115" s="57"/>
+      <c r="D115" s="71"/>
+      <c r="E115" s="72"/>
       <c r="F115" s="35"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B116" s="34"/>
       <c r="C116" s="16"/>
-      <c r="D116" s="56"/>
-      <c r="E116" s="57"/>
+      <c r="D116" s="71"/>
+      <c r="E116" s="72"/>
       <c r="F116" s="35"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B117" s="34"/>
       <c r="C117" s="16"/>
-      <c r="D117" s="56"/>
-      <c r="E117" s="57"/>
+      <c r="D117" s="71"/>
+      <c r="E117" s="72"/>
       <c r="F117" s="35"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B118" s="34"/>
       <c r="C118" s="16"/>
-      <c r="D118" s="56"/>
-      <c r="E118" s="57"/>
+      <c r="D118" s="71"/>
+      <c r="E118" s="72"/>
       <c r="F118" s="35"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B119" s="34"/>
       <c r="C119" s="16"/>
-      <c r="D119" s="56"/>
-      <c r="E119" s="57"/>
+      <c r="D119" s="71"/>
+      <c r="E119" s="72"/>
       <c r="F119" s="35"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B120" s="34"/>
       <c r="C120" s="16"/>
-      <c r="D120" s="56"/>
-      <c r="E120" s="57"/>
+      <c r="D120" s="71"/>
+      <c r="E120" s="72"/>
       <c r="F120" s="35"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B121" s="3"/>
       <c r="C121" s="1"/>
-      <c r="D121" s="56"/>
-      <c r="E121" s="57"/>
+      <c r="D121" s="71"/>
+      <c r="E121" s="72"/>
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B122" s="3"/>
       <c r="C122" s="1"/>
-      <c r="D122" s="56"/>
-      <c r="E122" s="57"/>
+      <c r="D122" s="71"/>
+      <c r="E122" s="72"/>
       <c r="F122" s="2"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B123" s="3"/>
       <c r="C123" s="1"/>
-      <c r="D123" s="56"/>
-      <c r="E123" s="57"/>
+      <c r="D123" s="71"/>
+      <c r="E123" s="72"/>
       <c r="F123" s="2"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B124" s="3"/>
       <c r="C124" s="1"/>
-      <c r="D124" s="56"/>
-      <c r="E124" s="57"/>
+      <c r="D124" s="71"/>
+      <c r="E124" s="72"/>
       <c r="F124" s="2"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B125" s="3"/>
       <c r="C125" s="1"/>
-      <c r="D125" s="56"/>
-      <c r="E125" s="57"/>
+      <c r="D125" s="71"/>
+      <c r="E125" s="72"/>
       <c r="F125" s="2"/>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B126" s="3"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="56"/>
-      <c r="E126" s="57"/>
+      <c r="D126" s="71"/>
+      <c r="E126" s="72"/>
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B127" s="3"/>
       <c r="C127" s="1"/>
-      <c r="D127" s="56"/>
-      <c r="E127" s="57"/>
+      <c r="D127" s="71"/>
+      <c r="E127" s="72"/>
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B128" s="3"/>
       <c r="C128" s="1"/>
-      <c r="D128" s="56"/>
-      <c r="E128" s="57"/>
+      <c r="D128" s="71"/>
+      <c r="E128" s="72"/>
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B129" s="3"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="56"/>
-      <c r="E129" s="57"/>
+      <c r="D129" s="71"/>
+      <c r="E129" s="72"/>
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B130" s="3"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="56"/>
-      <c r="E130" s="57"/>
+      <c r="D130" s="71"/>
+      <c r="E130" s="72"/>
       <c r="F130" s="2"/>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B131" s="3"/>
       <c r="C131" s="1"/>
-      <c r="D131" s="56"/>
-      <c r="E131" s="57"/>
+      <c r="D131" s="71"/>
+      <c r="E131" s="72"/>
       <c r="F131" s="2"/>
     </row>
     <row r="132" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B132" s="4"/>
       <c r="C132" s="5"/>
-      <c r="D132" s="60"/>
-      <c r="E132" s="61"/>
+      <c r="D132" s="75"/>
+      <c r="E132" s="76"/>
       <c r="F132" s="6"/>
     </row>
   </sheetData>
@@ -4263,7 +4611,6 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D20:E20"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
@@ -4272,6 +4619,7 @@
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
@@ -4285,10 +4633,11 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D20:E20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4313,12 +4662,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="2:5" ht="60.75" x14ac:dyDescent="0.15">
       <c r="B3" s="43" t="s">
@@ -4331,7 +4680,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="20.25" x14ac:dyDescent="0.15">
@@ -4436,12 +4785,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="12" t="s">
@@ -4544,44 +4893,44 @@
   <sheetData>
     <row r="1" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="75" t="s">
-        <v>70</v>
+      <c r="F3" s="87"/>
+      <c r="G3" s="90" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="69"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="70"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="10" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="75"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
@@ -4936,19 +5285,19 @@
       <c r="G33" s="9"/>
     </row>
     <row r="34" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="71"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="73"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
       <c r="G35" s="41"/>
     </row>
   </sheetData>
@@ -4994,63 +5343,63 @@
   <sheetData>
     <row r="1" spans="2:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:20" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="65" t="str">
+      <c r="B2" s="84" t="str">
         <f>'03_DiagnosticServicesList'!B5&amp;" Sub Function of Ecu Support"</f>
         <v>Diagnostic Session Control Sub Function of Ecu Support</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="67"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="86"/>
     </row>
     <row r="3" spans="2:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="75" t="s">
-        <v>70</v>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="90" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="52" t="str">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!B3)-1)</f>
         <v>DefaultSession</v>
@@ -5115,7 +5464,7 @@
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!I4)-1)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="75"/>
+      <c r="T4" s="90"/>
     </row>
     <row r="5" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="str">
@@ -5363,7 +5712,7 @@
   <dimension ref="B1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="B2:T12"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5382,63 +5731,63 @@
   <sheetData>
     <row r="1" spans="2:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:20" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="65" t="str">
+      <c r="B2" s="84" t="str">
         <f>'03_DiagnosticServicesList'!B6&amp;" Sub Function of Ecu Support"</f>
         <v>ECU Reset Sub Function of Ecu Support</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="67"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="86"/>
     </row>
     <row r="3" spans="2:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="75" t="s">
-        <v>70</v>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="90" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="52" t="str">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!B3)-1)</f>
         <v>DefaultSession</v>
@@ -5503,7 +5852,7 @@
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!I4)-1)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="75"/>
+      <c r="T4" s="90"/>
     </row>
     <row r="5" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
@@ -5742,158 +6091,191 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T12"/>
+  <dimension ref="B1:AA9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.75" customWidth="1"/>
+    <col min="4" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:20" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="65" t="str">
+    <row r="1" spans="2:27" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:27" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="95" t="str">
         <f>'03_DiagnosticServicesList'!B7&amp;" Sub Function of Ecu Support"</f>
         <v>Clear Diagnostic Information Sub Function of Ecu Support</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="67"/>
-    </row>
-    <row r="3" spans="2:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="69" t="s">
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="97"/>
+    </row>
+    <row r="3" spans="2:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="68" t="s">
+      <c r="C3" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68" t="s">
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="75" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="52" t="str">
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="B4" s="88"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="101" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="101" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="101" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="101" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="53" t="str">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!B3)-1)</f>
         <v>DefaultSession</v>
       </c>
-      <c r="E4" s="52" t="str">
+      <c r="L4" s="53" t="str">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!C3)-1)</f>
         <v>ProgrammingSession</v>
       </c>
-      <c r="F4" s="52" t="str">
+      <c r="M4" s="53" t="str">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!D3)-1)</f>
         <v>ExtendedSession</v>
       </c>
-      <c r="G4" s="52">
+      <c r="N4" s="53">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!E3)-1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="52">
+      <c r="O4" s="53">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!F3)-1)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="52">
+      <c r="P4" s="53">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!G3)-1)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="52">
+      <c r="Q4" s="53">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!H3)-1)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="52">
+      <c r="R4" s="53">
         <f>INDEX('01_DiagnosticSession'!$B$4:$B$11,COLUMN('01_DiagnosticSession'!I3)-1)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="52" t="str">
+      <c r="S4" s="53" t="str">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!B4)-1)</f>
         <v>SA_Level1</v>
       </c>
-      <c r="M4" s="52" t="str">
+      <c r="T4" s="53" t="str">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!C4)-1)</f>
         <v>SA_Level2</v>
       </c>
-      <c r="N4" s="52" t="str">
+      <c r="U4" s="53" t="str">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!D4)-1)</f>
         <v>SA_Level3</v>
       </c>
-      <c r="O4" s="52">
+      <c r="V4" s="53">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!E4)-1)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="52">
+      <c r="W4" s="53">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!F4)-1)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="52">
+      <c r="X4" s="53">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!G4)-1)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="52">
+      <c r="Y4" s="53">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!H4)-1)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="52">
+      <c r="Z4" s="53">
         <f>INDEX('02_SecurityAccess'!$B$4:$B$11,COLUMN('02_SecurityAccess'!I4)-1)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="75"/>
-    </row>
-    <row r="5" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>67</v>
-      </c>
+      <c r="AA4" s="90"/>
+    </row>
+    <row r="5" spans="2:27" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
         <v>31</v>
       </c>
@@ -5903,210 +6285,175 @@
       <c r="F5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="L5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="9"/>
-    </row>
-    <row r="6" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
-    </row>
-    <row r="7" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="9"/>
-    </row>
-    <row r="8" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="9"/>
-    </row>
-    <row r="9" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
-    </row>
-    <row r="10" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="9"/>
-    </row>
-    <row r="11" spans="2:20" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="9"/>
-    </row>
-    <row r="12" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="40"/>
-      <c r="T12" s="41"/>
+      <c r="S5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="9"/>
+    </row>
+    <row r="6" spans="2:27" ht="21" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="62"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="64"/>
+    </row>
+    <row r="7" spans="2:27" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="66"/>
+      <c r="V7" s="66"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="66"/>
+      <c r="Y7" s="66"/>
+      <c r="Z7" s="66"/>
+      <c r="AA7" s="67"/>
+    </row>
+    <row r="8" spans="2:27" ht="201" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="91" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="92"/>
+      <c r="O8" s="92"/>
+      <c r="P8" s="92"/>
+      <c r="Q8" s="92"/>
+      <c r="R8" s="92"/>
+      <c r="S8" s="92"/>
+      <c r="T8" s="92"/>
+      <c r="U8" s="92"/>
+      <c r="V8" s="92"/>
+      <c r="W8" s="92"/>
+      <c r="X8" s="92"/>
+      <c r="Y8" s="92"/>
+      <c r="Z8" s="92"/>
+      <c r="AA8" s="93"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="B2:T2"/>
+  <mergeCells count="7">
+    <mergeCell ref="B8:AA8"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="B2:AA2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="L3:S3"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="C3:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:S12 T5:T12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:AA6 C5:J5">
       <formula1>"Support,NotSupport"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>